<commit_message>
Transition matrix & figure
</commit_message>
<xml_diff>
--- a/data/Transition_data.xlsx
+++ b/data/Transition_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jenbaron\Documents\UBC\Research\PhD Thesis\Proposal\PhD Proposal\Analysis\PhDProposal\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{081AD812-AA96-475B-9282-54AEC0682E8D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76E0CAED-8655-49B5-A6C7-C61BA4CDEC3B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24930" windowHeight="11550" xr2:uid="{54B2ECD9-3359-4A4E-97C4-D3DD512799FB}"/>
   </bookViews>
@@ -402,8 +402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A86D627C-F04C-4F4C-955D-ACE0266896DB}">
   <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="G94" sqref="G94"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,10 +424,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>93</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -435,791 +435,791 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>95</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <v>96</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
+        <v>97</v>
+      </c>
+      <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
       <c r="C5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5</v>
+        <v>98</v>
       </c>
       <c r="B6" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="B7" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>7</v>
+        <v>62</v>
       </c>
       <c r="B8" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>8</v>
+        <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>9</v>
+        <v>64</v>
       </c>
       <c r="B10" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="B11" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="B12" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="B13" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>13</v>
+        <v>68</v>
       </c>
       <c r="B14" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="B15" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>15</v>
+        <v>70</v>
       </c>
       <c r="B16" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="B17" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>17</v>
+        <v>72</v>
       </c>
       <c r="B18" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>18</v>
+        <v>73</v>
       </c>
       <c r="B19" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>19</v>
+        <v>74</v>
       </c>
       <c r="B20" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>20</v>
+        <v>75</v>
       </c>
       <c r="B21" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>21</v>
+        <v>76</v>
       </c>
       <c r="B22" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C22" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>22</v>
+        <v>77</v>
       </c>
       <c r="B23" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>23</v>
+        <v>78</v>
       </c>
       <c r="B24" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>24</v>
+        <v>80</v>
       </c>
       <c r="B25" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C25" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>25</v>
+        <v>81</v>
       </c>
       <c r="B26" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C26" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>26</v>
+        <v>82</v>
       </c>
       <c r="B27" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C27" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>27</v>
+        <v>83</v>
       </c>
       <c r="B28" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C28" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>28</v>
+        <v>84</v>
       </c>
       <c r="B29" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C29" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>29</v>
+        <v>85</v>
       </c>
       <c r="B30" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C30" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>30</v>
+        <v>86</v>
       </c>
       <c r="B31" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C31" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>31</v>
+        <v>87</v>
       </c>
       <c r="B32" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C32" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>32</v>
+        <v>88</v>
       </c>
       <c r="B33" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C33" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>33</v>
+        <v>89</v>
       </c>
       <c r="B34" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C34" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>34</v>
+        <v>90</v>
       </c>
       <c r="B35" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C35" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>35</v>
+        <v>91</v>
       </c>
       <c r="B36" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C36" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>36</v>
+        <v>92</v>
       </c>
       <c r="B37" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C37" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>37</v>
+        <v>94</v>
       </c>
       <c r="B38" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C38" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>39</v>
+        <v>2</v>
       </c>
       <c r="B40" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="B41" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>41</v>
+        <v>4</v>
       </c>
       <c r="B42" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C42" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>42</v>
+        <v>5</v>
       </c>
       <c r="B43" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C43" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>43</v>
+        <v>6</v>
       </c>
       <c r="B44" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C44" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>44</v>
+        <v>7</v>
       </c>
       <c r="B45" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="B46" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="B47" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>47</v>
+        <v>10</v>
       </c>
       <c r="B48" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C48" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>48</v>
+        <v>11</v>
       </c>
       <c r="B49" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C49" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="B50" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="B51" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>51</v>
+        <v>14</v>
       </c>
       <c r="B52" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C52" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="B53" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C53" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="B54" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C54" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="B55" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C55" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="B56" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C56" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="B57" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C57" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="B58" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C58" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>58</v>
+        <v>21</v>
       </c>
       <c r="B59" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C59" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="B60" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C60" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="B61" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C61" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="B62" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C62" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="B63" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C63" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="B64" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C64" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="B65" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C65" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="B66" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C66" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="B67" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C67" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="B68" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C68" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="B69" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C69" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="B70" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C70" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="B71" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C71" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="B72" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C72" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="B73" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C73" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="B74" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C74" t="s">
         <v>7</v>
@@ -1227,10 +1227,10 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="B75" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C75" t="s">
         <v>7</v>
@@ -1238,10 +1238,10 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="B76" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C76" t="s">
         <v>7</v>
@@ -1249,10 +1249,10 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="B77" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C77" t="s">
         <v>7</v>
@@ -1260,10 +1260,10 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="B78" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C78" t="s">
         <v>7</v>
@@ -1271,258 +1271,261 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="B79" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C79" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="B80" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C80" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="B81" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C81" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>81</v>
+        <v>99</v>
       </c>
       <c r="B82" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C82" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="B83" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C83" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>83</v>
+        <v>22</v>
       </c>
       <c r="B84" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C84" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>84</v>
+        <v>23</v>
       </c>
       <c r="B85" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C85" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="B86" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C86" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>86</v>
+        <v>25</v>
       </c>
       <c r="B87" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C87" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>87</v>
+        <v>26</v>
       </c>
       <c r="B88" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C88" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>88</v>
+        <v>27</v>
       </c>
       <c r="B89" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C89" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>89</v>
+        <v>28</v>
       </c>
       <c r="B90" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C90" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="B91" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C91" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>91</v>
+        <v>31</v>
       </c>
       <c r="B92" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C92" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="B93" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C93" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="B94" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C94" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>94</v>
+        <v>34</v>
       </c>
       <c r="B95" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C95" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>95</v>
+        <v>35</v>
       </c>
       <c r="B96" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C96" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>96</v>
+        <v>36</v>
       </c>
       <c r="B97" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C97" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>97</v>
+        <v>37</v>
       </c>
       <c r="B98" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C98" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>98</v>
+        <v>38</v>
       </c>
       <c r="B99" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C99" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>99</v>
+        <v>39</v>
       </c>
       <c r="B100" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C100" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="B101" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C101" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:C101">
+    <sortCondition ref="B1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>